<commit_message>
Removed prints and updated README.md
</commit_message>
<xml_diff>
--- a/app/files/ThreeColorPalette/ThreeColorPalette-color-pallete.xlsx
+++ b/app/files/ThreeColorPalette/ThreeColorPalette-color-pallete.xlsx
@@ -41,164 +41,164 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00e2eeff"/>
-        <bgColor rgb="00e2eeff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00c9deff"/>
-        <bgColor rgb="00c9deff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00afcfff"/>
-        <bgColor rgb="00afcfff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0096c0ff"/>
-        <bgColor rgb="0096c0ff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0071a1e8"/>
-        <bgColor rgb="0071a1e8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004977bc"/>
-        <bgColor rgb="004977bc"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0029518e"/>
-        <bgColor rgb="0029518e"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00123160"/>
-        <bgColor rgb="00123160"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00041835"/>
-        <bgColor rgb="00041835"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fee2ff"/>
-        <bgColor rgb="00fee2ff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fec9ff"/>
-        <bgColor rgb="00fec9ff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fdafff"/>
-        <bgColor rgb="00fdafff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fd96ff"/>
-        <bgColor rgb="00fd96ff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00e671e8"/>
-        <bgColor rgb="00e671e8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ba49bc"/>
-        <bgColor rgb="00ba49bc"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="008d298e"/>
-        <bgColor rgb="008d298e"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005f1260"/>
-        <bgColor rgb="005f1260"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00340435"/>
-        <bgColor rgb="00340435"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00e2fff5"/>
-        <bgColor rgb="00e2fff5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00c9ffed"/>
-        <bgColor rgb="00c9ffed"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00afffe4"/>
-        <bgColor rgb="00afffe4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0096ffdc"/>
-        <bgColor rgb="0096ffdc"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0071e8c0"/>
-        <bgColor rgb="0071e8c0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0049bc96"/>
-        <bgColor rgb="0049bc96"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00298e6d"/>
-        <bgColor rgb="00298e6d"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00126046"/>
-        <bgColor rgb="00126046"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00043525"/>
-        <bgColor rgb="00043525"/>
+        <fgColor rgb="00bcf8ff"/>
+        <bgColor rgb="00bcf8ff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00a3f5ff"/>
+        <bgColor rgb="00a3f5ff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0089f3ff"/>
+        <bgColor rgb="0089f3ff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0070f0ff"/>
+        <bgColor rgb="0070f0ff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004ed8e8"/>
+        <bgColor rgb="004ed8e8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002cadbb"/>
+        <bgColor rgb="002cadbb"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0013828e"/>
+        <bgColor rgb="0013828e"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00035862"/>
+        <bgColor rgb="00035862"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00003035"/>
+        <bgColor rgb="00003035"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00efbcff"/>
+        <bgColor rgb="00efbcff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00e9a3ff"/>
+        <bgColor rgb="00e9a3ff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00e389ff"/>
+        <bgColor rgb="00e389ff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00dd70ff"/>
+        <bgColor rgb="00dd70ff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00c44ee8"/>
+        <bgColor rgb="00c44ee8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009a2cbb"/>
+        <bgColor rgb="009a2cbb"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0072138e"/>
+        <bgColor rgb="0072138e"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004c0362"/>
+        <bgColor rgb="004c0362"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00290035"/>
+        <bgColor rgb="00290035"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00e7ffbc"/>
+        <bgColor rgb="00e7ffbc"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00deffa3"/>
+        <bgColor rgb="00deffa3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00d5ff89"/>
+        <bgColor rgb="00d5ff89"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00cdff70"/>
+        <bgColor rgb="00cdff70"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00b2e84e"/>
+        <bgColor rgb="00b2e84e"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0089bb2c"/>
+        <bgColor rgb="0089bb2c"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00638e13"/>
+        <bgColor rgb="00638e13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00416203"/>
+        <bgColor rgb="00416203"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00223500"/>
+        <bgColor rgb="00223500"/>
       </patternFill>
     </fill>
     <fill>
@@ -215,32 +215,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00c6cad1"/>
-        <bgColor rgb="00c6cad1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0097a2b2"/>
-        <bgColor rgb="0097a2b2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00637084"/>
-        <bgColor rgb="00637084"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="003a4659"/>
-        <bgColor rgb="003a4659"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0019212d"/>
-        <bgColor rgb="0019212d"/>
+        <fgColor rgb="00c7d1d2"/>
+        <bgColor rgb="00c7d1d2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0097afb2"/>
+        <bgColor rgb="0097afb2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00648285"/>
+        <bgColor rgb="00648285"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003a5659"/>
+        <bgColor rgb="003a5659"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00182a2c"/>
+        <bgColor rgb="00182a2c"/>
       </patternFill>
     </fill>
     <fill>
@@ -248,218 +248,218 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00fcfffd"/>
-        <bgColor rgb="00fcfffd"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00e2ffe9"/>
-        <bgColor rgb="00e2ffe9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00c9ffd5"/>
-        <bgColor rgb="00c9ffd5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00afffc2"/>
-        <bgColor rgb="00afffc2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0085e29b"/>
-        <bgColor rgb="0085e29b"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0059b76f"/>
-        <bgColor rgb="0059b76f"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00358949"/>
-        <bgColor rgb="00358949"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="001a5b29"/>
-        <bgColor rgb="001a5b29"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00093012"/>
-        <bgColor rgb="00093012"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fffdfc"/>
-        <bgColor rgb="00fffdfc"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ffede2"/>
-        <bgColor rgb="00ffede2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ffddc9"/>
-        <bgColor rgb="00ffddc9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ffceaf"/>
-        <bgColor rgb="00ffceaf"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00e2a985"/>
-        <bgColor rgb="00e2a985"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00b77d59"/>
-        <bgColor rgb="00b77d59"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00895535"/>
-        <bgColor rgb="00895535"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005b331a"/>
-        <bgColor rgb="005b331a"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00301809"/>
-        <bgColor rgb="00301809"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fffcfc"/>
-        <bgColor rgb="00fffcfc"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ffe2e2"/>
-        <bgColor rgb="00ffe2e2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ffc9c9"/>
-        <bgColor rgb="00ffc9c9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ffafaf"/>
-        <bgColor rgb="00ffafaf"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00e28585"/>
-        <bgColor rgb="00e28585"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00b75959"/>
-        <bgColor rgb="00b75959"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00893535"/>
-        <bgColor rgb="00893535"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005b1a1a"/>
-        <bgColor rgb="005b1a1a"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00300909"/>
-        <bgColor rgb="00300909"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fcfdff"/>
-        <bgColor rgb="00fcfdff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00e2f3ff"/>
-        <bgColor rgb="00e2f3ff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00c9e9ff"/>
-        <bgColor rgb="00c9e9ff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00afdfff"/>
-        <bgColor rgb="00afdfff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0085bde2"/>
-        <bgColor rgb="0085bde2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005992b7"/>
-        <bgColor rgb="005992b7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00356889"/>
-        <bgColor rgb="00356889"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="001a415b"/>
-        <bgColor rgb="001a415b"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00092030"/>
-        <bgColor rgb="00092030"/>
+        <fgColor rgb="00d6ffdf"/>
+        <bgColor rgb="00d6ffdf"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00bcffcc"/>
+        <bgColor rgb="00bcffcc"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00a3ffb8"/>
+        <bgColor rgb="00a3ffb8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0089ffa5"/>
+        <bgColor rgb="0089ffa5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0063e281"/>
+        <bgColor rgb="0063e281"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003db65a"/>
+        <bgColor rgb="003db65a"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00218939"/>
+        <bgColor rgb="00218939"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000d5d1f"/>
+        <bgColor rgb="000d5d1f"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0001300c"/>
+        <bgColor rgb="0001300c"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffe5d6"/>
+        <bgColor rgb="00ffe5d6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffd6bc"/>
+        <bgColor rgb="00ffd6bc"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffc6a3"/>
+        <bgColor rgb="00ffc6a3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffb689"/>
+        <bgColor rgb="00ffb689"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00e29463"/>
+        <bgColor rgb="00e29463"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00b66c3d"/>
+        <bgColor rgb="00b66c3d"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00894921"/>
+        <bgColor rgb="00894921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005d2b0d"/>
+        <bgColor rgb="005d2b0d"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00301301"/>
+        <bgColor rgb="00301301"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffd6d6"/>
+        <bgColor rgb="00ffd6d6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffbcbc"/>
+        <bgColor rgb="00ffbcbc"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffa3a3"/>
+        <bgColor rgb="00ffa3a3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ff8989"/>
+        <bgColor rgb="00ff8989"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00e26363"/>
+        <bgColor rgb="00e26363"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00b63d3d"/>
+        <bgColor rgb="00b63d3d"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00892121"/>
+        <bgColor rgb="00892121"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005d0d0d"/>
+        <bgColor rgb="005d0d0d"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00300101"/>
+        <bgColor rgb="00300101"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00d6eeff"/>
+        <bgColor rgb="00d6eeff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00bce4ff"/>
+        <bgColor rgb="00bce4ff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00a3daff"/>
+        <bgColor rgb="00a3daff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0089d0ff"/>
+        <bgColor rgb="0089d0ff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0063b0e2"/>
+        <bgColor rgb="0063b0e2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003d86b6"/>
+        <bgColor rgb="003d86b6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00215f89"/>
+        <bgColor rgb="00215f89"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000d3d5d"/>
+        <bgColor rgb="000d3d5d"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00011d30"/>
+        <bgColor rgb="00011d30"/>
       </patternFill>
     </fill>
   </fills>
@@ -573,7 +573,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -588,7 +588,7 @@
     <xf numFmtId="0" fontId="1" fillId="50" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="59" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="59" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="68" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -606,10 +606,10 @@
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="51" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="51" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="60" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1119,31 +1119,31 @@
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Weight - 100
-HSB - (216, 11, 100)
-RGB - (226, 238, 255)
-HEX - #e2eeff</t>
+HSB - (186, 26, 100)
+RGB - (188, 248, 255)
+HEX - #bcf8ff</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Weight - 100
-HSB - (299, 11, 100)
-RGB - (254, 226, 255)
-HEX - #fee2ff</t>
+HSB - (286, 26, 100)
+RGB - (239, 188, 255)
+HEX - #efbcff</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Weight - 100
-HSB - (160, 11, 100)
-RGB - (226, 255, 245)
-HEX - #e2fff5</t>
+HSB - (81, 26, 100)
+RGB - (231, 255, 188)
+HEX - #e7ffbc</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
           <t>Weight - 100
-HSB - (216, 0, 100)
+HSB - (186, 0, 100)
 RGB - (255, 255, 255)
 HEX - #ffffff</t>
         </is>
@@ -1151,33 +1151,33 @@
       <c r="F2" s="5" t="inlineStr">
         <is>
           <t>Weight - 100
-HSB - (134, 1, 100)
-RGB - (252, 255, 253)
-HEX - #fcfffd</t>
+HSB - (134, 16, 100)
+RGB - (214, 255, 223)
+HEX - #d6ffdf</t>
         </is>
       </c>
       <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Weight - 100
-HSB - (23, 1, 100)
-RGB - (255, 253, 252)
-HEX - #fffdfc</t>
+HSB - (23, 16, 100)
+RGB - (255, 229, 214)
+HEX - #ffe5d6</t>
         </is>
       </c>
       <c r="H2" s="7" t="inlineStr">
         <is>
           <t>Weight - 100
-HSB - (0, 1, 100)
-RGB - (255, 252, 252)
-HEX - #fffcfc</t>
+HSB - (0, 16, 100)
+RGB - (255, 214, 214)
+HEX - #ffd6d6</t>
         </is>
       </c>
       <c r="I2" s="8" t="inlineStr">
         <is>
           <t>Weight - 100
-HSB - (204, 1, 100)
-RGB - (252, 253, 255)
-HEX - #fcfdff</t>
+HSB - (204, 16, 100)
+RGB - (214, 238, 255)
+HEX - #d6eeff</t>
         </is>
       </c>
     </row>
@@ -1185,31 +1185,31 @@
       <c r="B3" s="9" t="inlineStr">
         <is>
           <t>Weight - 200
-HSB - (216, 21, 100)
-RGB - (201, 222, 255)
-HEX - #c9deff</t>
+HSB - (186, 36, 100)
+RGB - (163, 245, 255)
+HEX - #a3f5ff</t>
         </is>
       </c>
       <c r="C3" s="10" t="inlineStr">
         <is>
           <t>Weight - 200
-HSB - (299, 21, 100)
-RGB - (254, 201, 255)
-HEX - #fec9ff</t>
+HSB - (286, 36, 100)
+RGB - (233, 163, 255)
+HEX - #e9a3ff</t>
         </is>
       </c>
       <c r="D3" s="11" t="inlineStr">
         <is>
           <t>Weight - 200
-HSB - (160, 21, 100)
-RGB - (201, 255, 237)
-HEX - #c9ffed</t>
+HSB - (81, 36, 100)
+RGB - (222, 255, 163)
+HEX - #deffa3</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
           <t>Weight - 200
-HSB - (216, 0, 100)
+HSB - (186, 0, 100)
 RGB - (255, 255, 255)
 HEX - #ffffff</t>
         </is>
@@ -1217,33 +1217,33 @@
       <c r="F3" s="12" t="inlineStr">
         <is>
           <t>Weight - 200
-HSB - (134, 11, 100)
-RGB - (226, 255, 233)
-HEX - #e2ffe9</t>
+HSB - (134, 26, 100)
+RGB - (188, 255, 204)
+HEX - #bcffcc</t>
         </is>
       </c>
       <c r="G3" s="13" t="inlineStr">
         <is>
           <t>Weight - 200
-HSB - (23, 11, 100)
-RGB - (255, 237, 226)
-HEX - #ffede2</t>
+HSB - (23, 26, 100)
+RGB - (255, 214, 188)
+HEX - #ffd6bc</t>
         </is>
       </c>
       <c r="H3" s="14" t="inlineStr">
         <is>
           <t>Weight - 200
-HSB - (0, 11, 100)
-RGB - (255, 226, 226)
-HEX - #ffe2e2</t>
+HSB - (0, 26, 100)
+RGB - (255, 188, 188)
+HEX - #ffbcbc</t>
         </is>
       </c>
       <c r="I3" s="15" t="inlineStr">
         <is>
           <t>Weight - 200
-HSB - (204, 11, 100)
-RGB - (226, 243, 255)
-HEX - #e2f3ff</t>
+HSB - (204, 26, 100)
+RGB - (188, 228, 255)
+HEX - #bce4ff</t>
         </is>
       </c>
     </row>
@@ -1251,31 +1251,31 @@
       <c r="B4" s="16" t="inlineStr">
         <is>
           <t>Weight - 300
-HSB - (216, 31, 100)
-RGB - (175, 207, 255)
-HEX - #afcfff</t>
+HSB - (186, 46, 100)
+RGB - (137, 243, 255)
+HEX - #89f3ff</t>
         </is>
       </c>
       <c r="C4" s="17" t="inlineStr">
         <is>
           <t>Weight - 300
-HSB - (299, 31, 100)
-RGB - (253, 175, 255)
-HEX - #fdafff</t>
+HSB - (286, 46, 100)
+RGB - (227, 137, 255)
+HEX - #e389ff</t>
         </is>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
           <t>Weight - 300
-HSB - (160, 31, 100)
-RGB - (175, 255, 228)
-HEX - #afffe4</t>
+HSB - (81, 46, 100)
+RGB - (213, 255, 137)
+HEX - #d5ff89</t>
         </is>
       </c>
       <c r="E4" s="19" t="inlineStr">
         <is>
           <t>Weight - 300
-HSB - (216, 0, 95)
+HSB - (186, 0, 95)
 RGB - (242, 242, 242)
 HEX - #f2f2f2</t>
         </is>
@@ -1283,33 +1283,33 @@
       <c r="F4" s="20" t="inlineStr">
         <is>
           <t>Weight - 300
-HSB - (134, 21, 100)
-RGB - (201, 255, 213)
-HEX - #c9ffd5</t>
+HSB - (134, 36, 100)
+RGB - (163, 255, 184)
+HEX - #a3ffb8</t>
         </is>
       </c>
       <c r="G4" s="21" t="inlineStr">
         <is>
           <t>Weight - 300
-HSB - (23, 21, 100)
-RGB - (255, 221, 201)
-HEX - #ffddc9</t>
+HSB - (23, 36, 100)
+RGB - (255, 198, 163)
+HEX - #ffc6a3</t>
         </is>
       </c>
       <c r="H4" s="22" t="inlineStr">
         <is>
           <t>Weight - 300
-HSB - (0, 21, 100)
-RGB - (255, 201, 201)
-HEX - #ffc9c9</t>
+HSB - (0, 36, 100)
+RGB - (255, 163, 163)
+HEX - #ffa3a3</t>
         </is>
       </c>
       <c r="I4" s="23" t="inlineStr">
         <is>
           <t>Weight - 300
-HSB - (204, 21, 100)
-RGB - (201, 233, 255)
-HEX - #c9e9ff</t>
+HSB - (204, 36, 100)
+RGB - (163, 218, 255)
+HEX - #a3daff</t>
         </is>
       </c>
     </row>
@@ -1317,65 +1317,65 @@
       <c r="B5" s="24" t="inlineStr">
         <is>
           <t>Weight - 400
-HSB - (216, 41, 100)
-RGB - (150, 192, 255)
-HEX - #96c0ff</t>
+HSB - (186, 56, 100)
+RGB - (112, 240, 255)
+HEX - #70f0ff</t>
         </is>
       </c>
       <c r="C5" s="25" t="inlineStr">
         <is>
           <t>Weight - 400
-HSB - (299, 41, 100)
-RGB - (253, 150, 255)
-HEX - #fd96ff</t>
+HSB - (286, 56, 100)
+RGB - (221, 112, 255)
+HEX - #dd70ff</t>
         </is>
       </c>
       <c r="D5" s="26" t="inlineStr">
         <is>
           <t>Weight - 400
-HSB - (160, 41, 100)
-RGB - (150, 255, 220)
-HEX - #96ffdc</t>
+HSB - (81, 56, 100)
+RGB - (205, 255, 112)
+HEX - #cdff70</t>
         </is>
       </c>
       <c r="E5" s="27" t="inlineStr">
         <is>
           <t>Weight - 400
-HSB - (216, 5, 82)
-RGB - (198, 202, 209)
-HEX - #c6cad1</t>
+HSB - (186, 5, 82.5)
+RGB - (199, 209, 210)
+HEX - #c7d1d2</t>
         </is>
       </c>
       <c r="F5" s="28" t="inlineStr">
         <is>
           <t>Weight - 400
-HSB - (134, 31, 100)
-RGB - (175, 255, 194)
-HEX - #afffc2</t>
+HSB - (134, 46, 100)
+RGB - (137, 255, 165)
+HEX - #89ffa5</t>
         </is>
       </c>
       <c r="G5" s="29" t="inlineStr">
         <is>
           <t>Weight - 400
-HSB - (23, 31, 100)
-RGB - (255, 206, 175)
-HEX - #ffceaf</t>
+HSB - (23, 46, 100)
+RGB - (255, 182, 137)
+HEX - #ffb689</t>
         </is>
       </c>
       <c r="H5" s="30" t="inlineStr">
         <is>
           <t>Weight - 400
-HSB - (0, 31, 100)
-RGB - (255, 175, 175)
-HEX - #ffafaf</t>
+HSB - (0, 46, 100)
+RGB - (255, 137, 137)
+HEX - #ff8989</t>
         </is>
       </c>
       <c r="I5" s="31" t="inlineStr">
         <is>
           <t>Weight - 400
-HSB - (204, 31, 100)
-RGB - (175, 223, 255)
-HEX - #afdfff</t>
+HSB - (204, 46, 100)
+RGB - (137, 208, 255)
+HEX - #89d0ff</t>
         </is>
       </c>
     </row>
@@ -1383,65 +1383,65 @@
       <c r="B6" s="32" t="inlineStr">
         <is>
           <t>Weight - 500
-HSB - (216, 51, 91)
-RGB - (113, 161, 232)
-HEX - #71a1e8</t>
+HSB - (186, 66, 91)
+RGB - (78, 216, 232)
+HEX - #4ed8e8</t>
         </is>
       </c>
       <c r="C6" s="33" t="inlineStr">
         <is>
           <t>Weight - 500
-HSB - (299, 51, 91)
-RGB - (230, 113, 232)
-HEX - #e671e8</t>
+HSB - (286, 66, 91)
+RGB - (196, 78, 232)
+HEX - #c44ee8</t>
         </is>
       </c>
       <c r="D6" s="34" t="inlineStr">
         <is>
           <t>Weight - 500
-HSB - (160, 51, 91)
-RGB - (113, 232, 192)
-HEX - #71e8c0</t>
+HSB - (81, 66, 91)
+RGB - (178, 232, 78)
+HEX - #b2e84e</t>
         </is>
       </c>
       <c r="E6" s="35" t="inlineStr">
         <is>
           <t>Weight - 500
-HSB - (216, 15, 70)
-RGB - (151, 162, 178)
-HEX - #97a2b2</t>
+HSB - (186, 15, 70)
+RGB - (151, 175, 178)
+HEX - #97afb2</t>
         </is>
       </c>
       <c r="F6" s="36" t="inlineStr">
         <is>
           <t>Weight - 500
-HSB - (134, 41, 89)
-RGB - (133, 226, 155)
-HEX - #85e29b</t>
+HSB - (134, 56, 89)
+RGB - (99, 226, 129)
+HEX - #63e281</t>
         </is>
       </c>
       <c r="G6" s="37" t="inlineStr">
         <is>
           <t>Weight - 500
-HSB - (23, 41, 89)
-RGB - (226, 169, 133)
-HEX - #e2a985</t>
+HSB - (23, 56, 89)
+RGB - (226, 148, 99)
+HEX - #e29463</t>
         </is>
       </c>
       <c r="H6" s="38" t="inlineStr">
         <is>
           <t>Weight - 500
-HSB - (0, 41, 89)
-RGB - (226, 133, 133)
-HEX - #e28585</t>
+HSB - (0, 56, 89)
+RGB - (226, 99, 99)
+HEX - #e26363</t>
         </is>
       </c>
       <c r="I6" s="39" t="inlineStr">
         <is>
           <t>Weight - 500
-HSB - (204, 41, 89)
-RGB - (133, 189, 226)
-HEX - #85bde2</t>
+HSB - (204, 56, 89)
+RGB - (99, 176, 226)
+HEX - #63b0e2</t>
         </is>
       </c>
     </row>
@@ -1449,65 +1449,65 @@
       <c r="B7" s="40" t="inlineStr">
         <is>
           <t>Weight - 600
-HSB - (216, 61, 74)
-RGB - (73, 119, 188)
-HEX - #4977bc</t>
+HSB - (186, 76, 73.5)
+RGB - (44, 173, 187)
+HEX - #2cadbb</t>
         </is>
       </c>
       <c r="C7" s="41" t="inlineStr">
         <is>
           <t>Weight - 600
-HSB - (299, 61, 74)
-RGB - (186, 73, 188)
-HEX - #ba49bc</t>
+HSB - (286, 76, 73.5)
+RGB - (154, 44, 187)
+HEX - #9a2cbb</t>
         </is>
       </c>
       <c r="D7" s="42" t="inlineStr">
         <is>
           <t>Weight - 600
-HSB - (160, 61, 74)
-RGB - (73, 188, 150)
-HEX - #49bc96</t>
+HSB - (81, 76, 73.5)
+RGB - (137, 187, 44)
+HEX - #89bb2c</t>
         </is>
       </c>
       <c r="E7" s="43" t="inlineStr">
         <is>
           <t>Weight - 600
-HSB - (216, 25, 52)
-RGB - (99, 112, 132)
-HEX - #637084</t>
+HSB - (186, 25, 52.5)
+RGB - (100, 130, 133)
+HEX - #648285</t>
         </is>
       </c>
       <c r="F7" s="44" t="inlineStr">
         <is>
           <t>Weight - 600
-HSB - (134, 51, 72)
-RGB - (89, 183, 111)
-HEX - #59b76f</t>
+HSB - (134, 66, 71.5)
+RGB - (61, 182, 90)
+HEX - #3db65a</t>
         </is>
       </c>
       <c r="G7" s="45" t="inlineStr">
         <is>
           <t>Weight - 600
-HSB - (23, 51, 72)
-RGB - (183, 125, 89)
-HEX - #b77d59</t>
+HSB - (23, 66, 71.5)
+RGB - (182, 108, 61)
+HEX - #b66c3d</t>
         </is>
       </c>
       <c r="H7" s="46" t="inlineStr">
         <is>
           <t>Weight - 600
-HSB - (0, 51, 72)
-RGB - (183, 89, 89)
-HEX - #b75959</t>
+HSB - (0, 66, 71.5)
+RGB - (182, 61, 61)
+HEX - #b63d3d</t>
         </is>
       </c>
       <c r="I7" s="47" t="inlineStr">
         <is>
           <t>Weight - 600
-HSB - (204, 51, 72)
-RGB - (89, 146, 183)
-HEX - #5992b7</t>
+HSB - (204, 66, 71.5)
+RGB - (61, 134, 182)
+HEX - #3d86b6</t>
         </is>
       </c>
     </row>
@@ -1515,65 +1515,65 @@
       <c r="B8" s="48" t="inlineStr">
         <is>
           <t>Weight - 700
-HSB - (216, 71, 56)
-RGB - (41, 81, 142)
-HEX - #29518e</t>
+HSB - (186, 86, 56)
+RGB - (19, 130, 142)
+HEX - #13828e</t>
         </is>
       </c>
       <c r="C8" s="49" t="inlineStr">
         <is>
           <t>Weight - 700
-HSB - (299, 71, 56)
-RGB - (141, 41, 142)
-HEX - #8d298e</t>
+HSB - (286, 86, 56)
+RGB - (114, 19, 142)
+HEX - #72138e</t>
         </is>
       </c>
       <c r="D8" s="50" t="inlineStr">
         <is>
           <t>Weight - 700
-HSB - (160, 71, 56)
-RGB - (41, 142, 109)
-HEX - #298e6d</t>
+HSB - (81, 86, 56)
+RGB - (99, 142, 19)
+HEX - #638e13</t>
         </is>
       </c>
       <c r="E8" s="51" t="inlineStr">
         <is>
           <t>Weight - 700
-HSB - (216, 35, 35)
-RGB - (58, 70, 89)
-HEX - #3a4659</t>
+HSB - (186, 35, 35)
+RGB - (58, 86, 89)
+HEX - #3a5659</t>
         </is>
       </c>
       <c r="F8" s="52" t="inlineStr">
         <is>
           <t>Weight - 700
-HSB - (134, 61, 54)
-RGB - (53, 137, 73)
-HEX - #358949</t>
+HSB - (134, 76, 54)
+RGB - (33, 137, 57)
+HEX - #218939</t>
         </is>
       </c>
       <c r="G8" s="53" t="inlineStr">
         <is>
           <t>Weight - 700
-HSB - (23, 61, 54)
-RGB - (137, 85, 53)
-HEX - #895535</t>
+HSB - (23, 76, 54)
+RGB - (137, 73, 33)
+HEX - #894921</t>
         </is>
       </c>
       <c r="H8" s="54" t="inlineStr">
         <is>
           <t>Weight - 700
-HSB - (0, 61, 54)
-RGB - (137, 53, 53)
-HEX - #893535</t>
+HSB - (0, 76, 54)
+RGB - (137, 33, 33)
+HEX - #892121</t>
         </is>
       </c>
       <c r="I8" s="55" t="inlineStr">
         <is>
           <t>Weight - 700
-HSB - (204, 61, 54)
-RGB - (53, 104, 137)
-HEX - #356889</t>
+HSB - (204, 76, 54)
+RGB - (33, 95, 137)
+HEX - #215f89</t>
         </is>
       </c>
     </row>
@@ -1581,65 +1581,65 @@
       <c r="B9" s="56" t="inlineStr">
         <is>
           <t>Weight - 800
-HSB - (216, 81, 38)
-RGB - (18, 49, 96)
-HEX - #123160</t>
+HSB - (186, 96, 38.5)
+RGB - (3, 88, 98)
+HEX - #035862</t>
         </is>
       </c>
       <c r="C9" s="57" t="inlineStr">
         <is>
           <t>Weight - 800
-HSB - (299, 81, 38)
-RGB - (95, 18, 96)
-HEX - #5f1260</t>
+HSB - (286, 96, 38.5)
+RGB - (76, 3, 98)
+HEX - #4c0362</t>
         </is>
       </c>
       <c r="D9" s="58" t="inlineStr">
         <is>
           <t>Weight - 800
-HSB - (160, 81, 38)
-RGB - (18, 96, 70)
-HEX - #126046</t>
+HSB - (81, 96, 38.5)
+RGB - (65, 98, 3)
+HEX - #416203</t>
         </is>
       </c>
       <c r="E9" s="59" t="inlineStr">
         <is>
           <t>Weight - 800
-HSB - (216, 45, 18)
-RGB - (25, 33, 45)
-HEX - #19212d</t>
+HSB - (186, 45, 17.5)
+RGB - (24, 42, 44)
+HEX - #182a2c</t>
         </is>
       </c>
       <c r="F9" s="60" t="inlineStr">
         <is>
           <t>Weight - 800
-HSB - (134, 71, 36)
-RGB - (26, 91, 41)
-HEX - #1a5b29</t>
+HSB - (134, 86, 36.5)
+RGB - (13, 93, 31)
+HEX - #0d5d1f</t>
         </is>
       </c>
       <c r="G9" s="61" t="inlineStr">
         <is>
           <t>Weight - 800
-HSB - (23, 71, 36)
-RGB - (91, 51, 26)
-HEX - #5b331a</t>
+HSB - (23, 86, 36.5)
+RGB - (93, 43, 13)
+HEX - #5d2b0d</t>
         </is>
       </c>
       <c r="H9" s="62" t="inlineStr">
         <is>
           <t>Weight - 800
-HSB - (0, 71, 36)
-RGB - (91, 26, 26)
-HEX - #5b1a1a</t>
+HSB - (0, 86, 36.5)
+RGB - (93, 13, 13)
+HEX - #5d0d0d</t>
         </is>
       </c>
       <c r="I9" s="63" t="inlineStr">
         <is>
           <t>Weight - 800
-HSB - (204, 71, 36)
-RGB - (26, 65, 91)
-HEX - #1a415b</t>
+HSB - (204, 86, 36.5)
+RGB - (13, 61, 93)
+HEX - #0d3d5d</t>
         </is>
       </c>
     </row>
@@ -1647,31 +1647,31 @@
       <c r="B10" s="64" t="inlineStr">
         <is>
           <t>Weight - 900
-HSB - (216, 91, 21)
-RGB - (4, 24, 53)
-HEX - #041835</t>
+HSB - (186, 100, 21)
+RGB - (0, 48, 53)
+HEX - #003035</t>
         </is>
       </c>
       <c r="C10" s="65" t="inlineStr">
         <is>
           <t>Weight - 900
-HSB - (299, 91, 21)
-RGB - (52, 4, 53)
-HEX - #340435</t>
+HSB - (286, 100, 21)
+RGB - (41, 0, 53)
+HEX - #290035</t>
         </is>
       </c>
       <c r="D10" s="66" t="inlineStr">
         <is>
           <t>Weight - 900
-HSB - (160, 91, 21)
-RGB - (4, 53, 37)
-HEX - #043525</t>
+HSB - (81, 100, 21)
+RGB - (34, 53, 0)
+HEX - #223500</t>
         </is>
       </c>
       <c r="E10" s="67" t="inlineStr">
         <is>
           <t>Weight - 900
-HSB - (216, 55, 0)
+HSB - (186, 55, 0)
 RGB - (0, 0, 0)
 HEX - #000000</t>
         </is>
@@ -1679,33 +1679,33 @@
       <c r="F10" s="68" t="inlineStr">
         <is>
           <t>Weight - 900
-HSB - (134, 81, 19)
-RGB - (9, 48, 18)
-HEX - #093012</t>
+HSB - (134, 96, 19)
+RGB - (1, 48, 12)
+HEX - #01300c</t>
         </is>
       </c>
       <c r="G10" s="69" t="inlineStr">
         <is>
           <t>Weight - 900
-HSB - (23, 81, 19)
-RGB - (48, 24, 9)
-HEX - #301809</t>
+HSB - (23, 96, 19)
+RGB - (48, 19, 1)
+HEX - #301301</t>
         </is>
       </c>
       <c r="H10" s="70" t="inlineStr">
         <is>
           <t>Weight - 900
-HSB - (0, 81, 19)
-RGB - (48, 9, 9)
-HEX - #300909</t>
+HSB - (0, 96, 19)
+RGB - (48, 1, 1)
+HEX - #300101</t>
         </is>
       </c>
       <c r="I10" s="71" t="inlineStr">
         <is>
           <t>Weight - 900
-HSB - (204, 81, 19)
-RGB - (9, 32, 48)
-HEX - #092030</t>
+HSB - (204, 96, 19)
+RGB - (1, 29, 48)
+HEX - #011d30</t>
         </is>
       </c>
     </row>

</xml_diff>